<commit_message>
Updated configuration files for visiumhd datasets
</commit_message>
<xml_diff>
--- a/datasets/10x_visiumhd_mouse_brain.xlsx
+++ b/datasets/10x_visiumhd_mouse_brain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\andpe\Documents\GitLab\scrnaseq2\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92545B2-D4FB-49A2-9DC7-0A13B83C3D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1D6769-A33D-4A90-A142-9CA0979A68B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>sample</t>
   </si>
@@ -69,7 +69,10 @@
     <t>mouse_brain</t>
   </si>
   <si>
-    <t>datasets/10x_visiumhd_brain/segmented_outputs/filtered_feature_bc_matrix.h5</t>
+    <t>datasets/10x_visiumhd_mouse_brain/metrics_summary.csv</t>
+  </si>
+  <si>
+    <t>datasets/10x_visiumhd_mouse_brain/segmented_outputs/filtered_feature_cell_matrix.h5</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -497,6 +500,9 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="I2" t="s">

</xml_diff>

<commit_message>
Fixed technology in visiumhd dataset files
</commit_message>
<xml_diff>
--- a/datasets/10x_visiumhd_mouse_brain.xlsx
+++ b/datasets/10x_visiumhd_mouse_brain.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\andpe\Documents\GitLab\scrnaseq2\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1D6769-A33D-4A90-A142-9CA0979A68B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65F1E0C-D2E5-4794-8A6E-C5006CC4FD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>barcode_suffix</t>
   </si>
   <si>
-    <t>10x_visium</t>
-  </si>
-  <si>
     <t>RNA</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>datasets/10x_visiumhd_mouse_brain/segmented_outputs/filtered_feature_cell_matrix.h5</t>
+  </si>
+  <si>
+    <t>10x_visiumhd</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -488,25 +488,25 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>